<commit_message>
Add figure saving, UTF encoding, README updates, folder creation fixes
</commit_message>
<xml_diff>
--- a/Parameters/country_parameters.xlsx
+++ b/Parameters/country_parameters.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mans3904/Documents/GitHub/GEOH2-private/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lahert5576\PycharmProjects\GeoH2\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{398819B3-C281-7544-A826-A9A0680DB2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEFBFBC-AA6E-484A-92FF-242DBF2FF926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21360" yWindow="-23280" windowWidth="28040" windowHeight="16760" xr2:uid="{DABDD650-3650-EB49-9A3D-C99E53AAB8F9}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="12645" xr2:uid="{DABDD650-3650-EB49-9A3D-C99E53AAB8F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -41,9 +30,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Kenya</t>
-  </si>
-  <si>
     <t>Solar interest rate</t>
   </si>
   <si>
@@ -68,19 +54,25 @@
     <t>Infrastructure lifetime (years)</t>
   </si>
   <si>
-    <t>Tanzania</t>
-  </si>
-  <si>
     <t>Electricity price (euros/kWh)</t>
   </si>
   <si>
     <t>Heat price (euros/kWh)</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -110,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,123 +422,124 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.125" customWidth="1"/>
+    <col min="2" max="2" width="37.125" customWidth="1"/>
+    <col min="3" max="3" width="26.125" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="24.625" customWidth="1"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
+    <col min="11" max="11" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
       <c r="B2">
-        <v>0.08</v>
+        <v>0.10465000000000001</v>
       </c>
       <c r="C2">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="D2">
-        <v>0.05</v>
+        <v>5.7890216323739932E-2</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2">
-        <v>7.0000000000000007E-2</v>
+        <v>5.7890216323739932E-2</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2">
-        <v>7.0000000000000007E-2</v>
+        <v>5.7890216323739932E-2</v>
       </c>
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2">
-        <v>0.03</v>
+      <c r="J2" s="1">
+        <v>5.7890216323739932E-2</v>
       </c>
       <c r="K2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>0.08</v>
+        <v>0.10465000000000001</v>
       </c>
       <c r="C3">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="D3">
-        <v>0.05</v>
+        <v>5.7890216323739932E-2</v>
       </c>
       <c r="E3">
         <v>20</v>
       </c>
       <c r="F3">
-        <v>7.0000000000000007E-2</v>
+        <v>5.7890216323739932E-2</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3">
-        <v>7.0000000000000007E-2</v>
+        <v>5.7890216323739932E-2</v>
       </c>
       <c r="I3">
         <v>20</v>
       </c>
-      <c r="J3">
-        <v>0.03</v>
+      <c r="J3" s="1">
+        <v>5.7890216323739932E-2</v>
       </c>
       <c r="K3">
         <v>50</v>

</xml_diff>

<commit_message>
Merging Alycia's code edits with Claire's latest push
</commit_message>
<xml_diff>
--- a/Parameters/country_parameters.xlsx
+++ b/Parameters/country_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lahert5576\PycharmProjects\GeoH2\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5576_ox_ac_uk/Documents/CCG/GEOH2/ETH Hydrogen Collaboration/Inputs and results v9 2023-08-11/Export - De-risked/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEFBFBC-AA6E-484A-92FF-242DBF2FF926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{00534948-BCBD-704C-99CC-18B96561D95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BE0B69B-8640-4B51-B832-BA00B15AE788}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="12645" xr2:uid="{DABDD650-3650-EB49-9A3D-C99E53AAB8F9}"/>
+    <workbookView xWindow="4890" yWindow="1680" windowWidth="28800" windowHeight="15345" xr2:uid="{DABDD650-3650-EB49-9A3D-C99E53AAB8F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -70,9 +79,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000000000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -102,9 +108,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,7 +427,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -433,10 +438,8 @@
     <col min="4" max="4" width="25.5" customWidth="1"/>
     <col min="5" max="5" width="24.625" customWidth="1"/>
     <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.375" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.625" customWidth="1"/>
-    <col min="10" max="10" width="28.5" customWidth="1"/>
+    <col min="7" max="8" width="25.375" customWidth="1"/>
+    <col min="9" max="10" width="24.625" customWidth="1"/>
     <col min="11" max="11" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -486,25 +489,25 @@
         <v>0.02</v>
       </c>
       <c r="D2">
-        <v>5.7890216323739932E-2</v>
+        <v>6.6053564606404797E-2</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2">
-        <v>5.7890216323739932E-2</v>
+        <v>6.6053564606404797E-2</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2">
-        <v>5.7890216323739932E-2</v>
+        <v>6.6053564606404797E-2</v>
       </c>
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2" s="1">
-        <v>5.7890216323739932E-2</v>
+      <c r="J2">
+        <v>5.9635333081896211E-2</v>
       </c>
       <c r="K2">
         <v>50</v>
@@ -521,25 +524,25 @@
         <v>0.02</v>
       </c>
       <c r="D3">
-        <v>5.7890216323739932E-2</v>
+        <v>6.6053564606404797E-2</v>
       </c>
       <c r="E3">
         <v>20</v>
       </c>
       <c r="F3">
-        <v>5.7890216323739932E-2</v>
+        <v>6.6053564606404797E-2</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3">
-        <v>5.7890216323739932E-2</v>
+        <v>6.6053564606404797E-2</v>
       </c>
       <c r="I3">
         <v>20</v>
       </c>
-      <c r="J3" s="1">
-        <v>5.7890216323739932E-2</v>
+      <c r="J3">
+        <v>5.9635333081896211E-2</v>
       </c>
       <c r="K3">
         <v>50</v>

</xml_diff>

<commit_message>
Alycia's latest edits - ensuring same code for model run split with Claire
</commit_message>
<xml_diff>
--- a/Parameters/country_parameters.xlsx
+++ b/Parameters/country_parameters.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5576_ox_ac_uk/Documents/CCG/GEOH2/ETH Hydrogen Collaboration/Inputs and results v9 2023-08-11/Export - De-risked/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5576_ox_ac_uk/Documents/CCG/GEOH2/ETH Hydrogen Collaboration/Inputs and results v12 2023-09-05/kenya-local-derisked/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{00534948-BCBD-704C-99CC-18B96561D95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BE0B69B-8640-4B51-B832-BA00B15AE788}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{3169747F-BB5E-B44C-AD55-C824E8A6DA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04261381-5834-4069-BCF1-74131D9EE601}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="1680" windowWidth="28800" windowHeight="15345" xr2:uid="{DABDD650-3650-EB49-9A3D-C99E53AAB8F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DABDD650-3650-EB49-9A3D-C99E53AAB8F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,11 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Country</t>
   </si>
   <si>
+    <t>Kenya</t>
+  </si>
+  <si>
     <t>Solar interest rate</t>
   </si>
   <si>
@@ -63,6 +67,9 @@
     <t>Infrastructure lifetime (years)</t>
   </si>
   <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
     <t>Electricity price (euros/kWh)</t>
   </si>
   <si>
@@ -70,6 +77,111 @@
   </si>
   <si>
     <t>Namibia</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>São Tomé and Príncipe</t>
+  </si>
+  <si>
+    <t>Congo, Democratic Republic Of</t>
+  </si>
+  <si>
+    <t>Congo, Republic of</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Niger</t>
   </si>
   <si>
     <t>Other</t>
@@ -79,6 +191,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -88,15 +203,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -104,12 +225,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,6 +278,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,19 +584,14 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.125" customWidth="1"/>
-    <col min="2" max="2" width="37.125" customWidth="1"/>
-    <col min="3" max="3" width="26.125" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="24.625" customWidth="1"/>
-    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="25.375" customWidth="1"/>
-    <col min="9" max="10" width="24.625" customWidth="1"/>
+    <col min="1" max="8" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="24.625" customWidth="1"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
     <col min="11" max="11" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -448,66 +600,66 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.10465000000000001</v>
+        <v>4.914000000000001E-2</v>
       </c>
       <c r="C2">
         <v>0.02</v>
       </c>
       <c r="D2">
-        <v>6.6053564606404797E-2</v>
+        <v>9.5866064606404802E-2</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2">
-        <v>6.6053564606404797E-2</v>
+        <v>9.5866064606404802E-2</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2">
-        <v>6.6053564606404797E-2</v>
+        <v>9.5866064606404802E-2</v>
       </c>
       <c r="I2">
         <v>20</v>
       </c>
       <c r="J2">
-        <v>5.9635333081896211E-2</v>
+        <v>6.4928564999999994E-2</v>
       </c>
       <c r="K2">
         <v>50</v>
@@ -515,37 +667,356 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B3">
-        <v>0.10465000000000001</v>
+        <v>4.914000000000001E-2</v>
       </c>
       <c r="C3">
         <v>0.02</v>
       </c>
       <c r="D3">
-        <v>6.6053564606404797E-2</v>
+        <v>9.5866064606404802E-2</v>
       </c>
       <c r="E3">
         <v>20</v>
       </c>
       <c r="F3">
-        <v>6.6053564606404797E-2</v>
+        <v>9.5866064606404802E-2</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3">
-        <v>6.6053564606404797E-2</v>
+        <v>9.5866064606404802E-2</v>
       </c>
       <c r="I3">
         <v>20</v>
       </c>
       <c r="J3">
-        <v>5.9635333081896211E-2</v>
+        <v>6.4928564999999994E-2</v>
       </c>
       <c r="K3">
         <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8B24D7-04E6-934C-8675-2FD45940E249}">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3">
+        <v>7.7116064606404716E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="4">
+        <v>8.1803564606404797E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3">
+        <v>8.1803564606404797E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4">
+        <v>7.7116064606404716E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8.6491064606404794E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
+        <v>8.6491064606404794E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3">
+        <v>8.6491064606404794E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4">
+        <v>8.6491064606404794E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8.6491064606404794E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4">
+        <v>9.1178564606404805E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3">
+        <v>8.6491064606404794E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4">
+        <v>9.5866064606404802E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8.6491064606404794E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>9.1178564606404805E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3">
+        <v>9.1178564606404805E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="4">
+        <v>9.5866064606404802E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3">
+        <v>9.1178564606404805E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4">
+        <v>9.1178564606404805E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3">
+        <v>8.6491064606404794E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4">
+        <v>9.5866064606404802E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3">
+        <v>9.1178564606404805E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.1005535646064048</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="3">
+        <v>9.5866064606404802E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <v>9.5866064606404802E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="3">
+        <v>9.5866064606404802E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.1005535646064048</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.1005535646064048</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.1005535646064048</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3">
+        <v>9.5866064606404802E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="4">
+        <v>9.5866064606404802E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.1052410646064048</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.1005535646064048</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.1005535646064048</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.1052410646064048</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.1005535646064048</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0.1052410646064048</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.1052410646064048</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.10992856460640443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add case study parameters and parameter ref tables to readme.
</commit_message>
<xml_diff>
--- a/Parameters/country_parameters.xlsx
+++ b/Parameters/country_parameters.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5576_ox_ac_uk/Documents/CCG/GEOH2/ETHCollab/MethodsX/Case study option 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5576_ox_ac_uk/Documents/CCG/GEOH2/ETHCollab/HydrogenRuns/v15_2024-01-03/interest_6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{1CFD0A5C-DDE5-1246-8F99-DF1D952BCB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37320173-D4A3-4920-ABF3-130A22E0F991}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{9F3E4EC1-8BA9-8B46-891F-3450F85F2F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15AE0AC0-A426-4233-A257-5A2872D45AFD}"/>
   <bookViews>
-    <workbookView xWindow="37060" yWindow="500" windowWidth="14400" windowHeight="9660" xr2:uid="{DABDD650-3650-EB49-9A3D-C99E53AAB8F9}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="16200" windowHeight="9270" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,34 +40,34 @@
     <t>Country</t>
   </si>
   <si>
+    <t>Electricity price (euros/kWh)</t>
+  </si>
+  <si>
+    <t>Heat price (euros/kWh)</t>
+  </si>
+  <si>
     <t>Solar interest rate</t>
   </si>
   <si>
+    <t>Solar lifetime (years)</t>
+  </si>
+  <si>
     <t>Wind interest rate</t>
   </si>
   <si>
+    <t>Wind lifetime (years)</t>
+  </si>
+  <si>
     <t>Plant interest rate</t>
   </si>
   <si>
+    <t>Plant lifetime (years)</t>
+  </si>
+  <si>
     <t>Infrastructure interest rate</t>
   </si>
   <si>
-    <t>Solar lifetime (years)</t>
-  </si>
-  <si>
-    <t>Wind lifetime (years)</t>
-  </si>
-  <si>
-    <t>Plant lifetime (years)</t>
-  </si>
-  <si>
     <t>Infrastructure lifetime (years)</t>
-  </si>
-  <si>
-    <t>Electricity price (euros/kWh)</t>
-  </si>
-  <si>
-    <t>Heat price (euros/kWh)</t>
   </si>
   <si>
     <t>Namibia</t>
@@ -423,126 +424,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766D5AAE-F1F5-A043-943F-C41FD6FD6FED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A655327-FB0F-D040-A870-A9F18A82B881}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="24.375" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="26.125" customWidth="1"/>
+    <col min="7" max="7" width="19.875" customWidth="1"/>
+    <col min="8" max="8" width="20.125" customWidth="1"/>
+    <col min="9" max="9" width="18.125" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2">
-        <v>0.10465000000000001</v>
+        <v>0.108</v>
       </c>
       <c r="C2">
         <v>0.02</v>
       </c>
       <c r="D2">
-        <v>6.1178564606404806E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2">
-        <v>6.1178564606404806E-2</v>
+        <v>0.06</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2">
-        <v>6.1178564606404806E-2</v>
+        <v>0.06</v>
       </c>
       <c r="I2">
         <v>20</v>
       </c>
       <c r="J2">
-        <v>6.1178564606404806E-2</v>
+        <v>0.06</v>
       </c>
       <c r="K2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
-        <v>0.10465000000000001</v>
+        <v>0.108</v>
       </c>
       <c r="C3">
         <v>0.02</v>
       </c>
       <c r="D3">
-        <v>6.1178564606404806E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E3">
         <v>20</v>
       </c>
       <c r="F3">
-        <v>6.1178564606404806E-2</v>
+        <v>0.06</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3">
-        <v>6.1178564606404806E-2</v>
+        <v>0.06</v>
       </c>
       <c r="I3">
         <v>20</v>
       </c>
       <c r="J3">
-        <v>6.1178564606404806E-2</v>
+        <v>0.06</v>
       </c>
       <c r="K3">
         <v>50</v>

</xml_diff>